<commit_message>
Alterações e melhorias no projeto
</commit_message>
<xml_diff>
--- a/Disparador sem Anexo/src/static/Enviar E-mails.xlsx
+++ b/Disparador sem Anexo/src/static/Enviar E-mails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Códigos\Projeto-Envio-Email\Disparador sem Anexo\src\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5BFF2-74E0-4939-8523-2FDB3A6DE208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769B549D-09D0-4C75-930A-7537017E47EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>E-mail</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Protocolo</t>
-  </si>
-  <si>
-    <t>Produto</t>
-  </si>
-  <si>
-    <t>STATUS</t>
+    <t>INDICADOR</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -397,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="A2:E4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,6 +423,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementação de redirecionamento, correção de bugs e melhoria no código
</commit_message>
<xml_diff>
--- a/Disparador sem Anexo/src/static/Enviar E-mails.xlsx
+++ b/Disparador sem Anexo/src/static/Enviar E-mails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Códigos\Projeto-Envio-Email\Disparador sem Anexo\src\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suporte.2.WEBCERTIFICADOS\Desktop\Projetos do Github\Projeto-Envio-Email\Disparador sem Anexo\src\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100E543A-AB0F-4C08-B20B-E100A1720FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FDB0E6-0095-42C0-A69E-2A1EDB28FF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>